<commit_message>
D by d to 100. Implemented 2MW system.
</commit_message>
<xml_diff>
--- a/inputData/Eco.xlsx
+++ b/inputData/Eco.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27425"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27231"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://polimi365-my.sharepoint.com/personal/10791792_polimi_it/Documents/2024-04 Economic model/EcoModel/inputData/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\PhD\GitHubRepo\EcoModel\inputData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="414" documentId="11_F25DC773A252ABDACC1048D3711B4E545ADE58EC" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C532B7DD-C864-489B-ABCC-5451FE20F1F2}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DE1177CA-2844-43CD-B347-4B0996FC1EED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="kite" sheetId="3" r:id="rId1"/>
@@ -225,8 +225,8 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
-    <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="164" formatCode="_(* #,##0.000_);_(* \(#,##0.000\);_(* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="164" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="165" formatCode="_(* #,##0.000_);_(* \(#,##0.000\);_(* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
@@ -263,12 +263,12 @@
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -556,13 +556,13 @@
       <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="29.08984375" customWidth="1"/>
-    <col min="2" max="2" width="17.453125" customWidth="1"/>
+    <col min="1" max="1" width="29.140625" customWidth="1"/>
+    <col min="2" max="2" width="17.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>19</v>
       </c>
@@ -570,7 +570,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -578,7 +578,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -586,7 +586,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>3</v>
       </c>
@@ -594,7 +594,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>4</v>
       </c>
@@ -602,7 +602,7 @@
         <v>3.6</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>5</v>
       </c>
@@ -610,7 +610,7 @@
         <v>0.75</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>6</v>
       </c>
@@ -618,7 +618,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>29</v>
       </c>
@@ -626,7 +626,7 @@
         <v>0.56999999999999995</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>30</v>
       </c>
@@ -634,7 +634,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>31</v>
       </c>
@@ -642,7 +642,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>31</v>
       </c>
@@ -650,7 +650,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>32</v>
       </c>
@@ -658,7 +658,7 @@
         <v>15000</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B14" s="1"/>
     </row>
   </sheetData>
@@ -670,17 +670,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CF4AD09E-FDEF-4026-AC1D-93146C2A9B86}">
   <dimension ref="A1:H8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="27.81640625" customWidth="1"/>
-    <col min="2" max="2" width="23.453125" customWidth="1"/>
+    <col min="1" max="1" width="27.85546875" customWidth="1"/>
+    <col min="2" max="2" width="23.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>33</v>
       </c>
@@ -689,7 +689,7 @@
       </c>
       <c r="H1" s="1"/>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>7</v>
       </c>
@@ -698,7 +698,7 @@
       </c>
       <c r="H2" s="1"/>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>8</v>
       </c>
@@ -706,7 +706,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>9</v>
       </c>
@@ -714,7 +714,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>10</v>
       </c>
@@ -722,7 +722,7 @@
         <v>0.85</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>56</v>
       </c>
@@ -730,7 +730,7 @@
         <v>6.5</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>57</v>
       </c>
@@ -738,7 +738,7 @@
         <v>2.6</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>58</v>
       </c>
@@ -755,25 +755,25 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B5144ACA-6792-40EA-A07E-EF86968317B7}">
   <dimension ref="A1:B31"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G28" sqref="G28"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F16" sqref="F16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="24.54296875" customWidth="1"/>
+    <col min="1" max="1" width="24.5703125" customWidth="1"/>
     <col min="2" max="2" width="11" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>11</v>
       </c>
       <c r="B1">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>12</v>
       </c>
@@ -781,7 +781,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>13</v>
       </c>
@@ -789,7 +789,7 @@
         <v>2700</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>14</v>
       </c>
@@ -797,7 +797,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>15</v>
       </c>
@@ -805,7 +805,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>16</v>
       </c>
@@ -813,7 +813,7 @@
         <v>7850</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>17</v>
       </c>
@@ -821,7 +821,7 @@
         <v>500</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>51</v>
       </c>
@@ -829,7 +829,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>52</v>
       </c>
@@ -837,7 +837,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>18</v>
       </c>
@@ -845,7 +845,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>34</v>
       </c>
@@ -853,7 +853,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>35</v>
       </c>
@@ -861,7 +861,7 @@
         <v>12.9</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>36</v>
       </c>
@@ -869,7 +869,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>37</v>
       </c>
@@ -877,7 +877,7 @@
         <v>0.71</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>20</v>
       </c>
@@ -885,7 +885,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>38</v>
       </c>
@@ -893,7 +893,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>39</v>
       </c>
@@ -901,7 +901,7 @@
         <v>12.4</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>41</v>
       </c>
@@ -909,7 +909,7 @@
         <v>2.2999999999999998</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>40</v>
       </c>
@@ -917,7 +917,7 @@
         <v>3400</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>42</v>
       </c>
@@ -925,7 +925,7 @@
         <v>60000</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>43</v>
       </c>
@@ -934,7 +934,7 @@
         <v>1000000</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>44</v>
       </c>
@@ -942,7 +942,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>45</v>
       </c>
@@ -950,7 +950,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>21</v>
       </c>
@@ -958,7 +958,7 @@
         <v>0.125</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>46</v>
       </c>
@@ -966,7 +966,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>47</v>
       </c>
@@ -974,7 +974,7 @@
         <v>30000</v>
       </c>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>22</v>
       </c>
@@ -982,7 +982,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>48</v>
       </c>
@@ -990,7 +990,7 @@
         <v>1200</v>
       </c>
     </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>49</v>
       </c>
@@ -998,7 +998,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>50</v>
       </c>
@@ -1006,7 +1006,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>23</v>
       </c>
@@ -1028,12 +1028,12 @@
       <selection activeCell="H14" sqref="H14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="17.54296875" customWidth="1"/>
+    <col min="1" max="1" width="17.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>24</v>
       </c>
@@ -1041,7 +1041,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>25</v>
       </c>
@@ -1049,7 +1049,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>26</v>
       </c>
@@ -1057,7 +1057,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>27</v>
       </c>
@@ -1065,7 +1065,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>28</v>
       </c>
@@ -1086,7 +1086,7 @@
       <selection activeCell="D35" sqref="D35"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1100,12 +1100,12 @@
       <selection activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="27.26953125" customWidth="1"/>
+    <col min="1" max="1" width="27.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>53</v>
       </c>
@@ -1113,7 +1113,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>54</v>
       </c>
@@ -1121,7 +1121,7 @@
         <v>-1.2</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>55</v>
       </c>

</xml_diff>

<commit_message>
USe D by d of 90. Use steel for winch.
</commit_message>
<xml_diff>
--- a/inputData/Eco.xlsx
+++ b/inputData/Eco.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\PhD\GitHubRepo\EcoModel\inputData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DE1177CA-2844-43CD-B347-4B0996FC1EED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6D9242BC-CA45-46E3-AFED-CD814D054A73}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -756,7 +756,7 @@
   <dimension ref="A1:B31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F16" sqref="F16"/>
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -770,7 +770,7 @@
         <v>11</v>
       </c>
       <c r="B1">
-        <v>100</v>
+        <v>90</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
@@ -826,7 +826,7 @@
         <v>51</v>
       </c>
       <c r="B8">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Kite avionics cost to commercial scale
</commit_message>
<xml_diff>
--- a/inputData/Eco.xlsx
+++ b/inputData/Eco.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\PhD\GitHubRepo\EcoModel\inputData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6D9242BC-CA45-46E3-AFED-CD814D054A73}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ADE4943C-9F95-4EDE-95CA-B0881E12E962}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="kite" sheetId="3" r:id="rId1"/>
@@ -552,8 +552,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{44B3DA40-233C-46C9-8316-C78F88E0B4B1}">
   <dimension ref="A1:B14"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F13" sqref="F13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G10" sqref="G10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -655,7 +655,7 @@
         <v>32</v>
       </c>
       <c r="B12" s="1">
-        <v>15000</v>
+        <v>150000</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
@@ -755,7 +755,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B5144ACA-6792-40EA-A07E-EF86968317B7}">
   <dimension ref="A1:B31"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Correct tether stress equation, correct ultracap equation, update system inputs to operate at 0.6GPa of tether stress
</commit_message>
<xml_diff>
--- a/inputData/Eco.xlsx
+++ b/inputData/Eco.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\PhD\GitHubRepo\EcoModel\inputData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ADE4943C-9F95-4EDE-95CA-B0881E12E962}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{151D6B61-07EB-4DB0-8EF1-29A5F1296ECE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="kite" sheetId="3" r:id="rId1"/>
@@ -552,7 +552,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{44B3DA40-233C-46C9-8316-C78F88E0B4B1}">
   <dimension ref="A1:B14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G10" sqref="G10"/>
     </sheetView>
   </sheetViews>
@@ -755,8 +755,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B5144ACA-6792-40EA-A07E-EF86968317B7}">
   <dimension ref="A1:B31"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="P17" sqref="P17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>